<commit_message>
feat: added more images
</commit_message>
<xml_diff>
--- a/tests/event_imageurls.xlsx
+++ b/tests/event_imageurls.xlsx
@@ -1192,9 +1192,9 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1743,74 +1743,94 @@
       <c r="H30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="n">
+      <c r="A31" s="17" t="n">
         <v>44944.8757384838</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="19" t="s">
         <v>83</v>
       </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="n">
+      <c r="A32" s="17" t="n">
         <v>44944.8759675232</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="19" t="s">
         <v>86</v>
       </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="n">
+      <c r="A33" s="17" t="n">
         <v>44944.8769399653</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="19" t="s">
         <v>89</v>
       </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="n">
+      <c r="A34" s="17" t="n">
         <v>44944.8771110417</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="19" t="s">
         <v>91</v>
       </c>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="n">
+      <c r="A35" s="17" t="n">
         <v>44944.8774606019</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="19" t="s">
         <v>93</v>
       </c>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="n">

</xml_diff>

<commit_message>
feat: case insensitive search
</commit_message>
<xml_diff>
--- a/tests/event_imageurls.xlsx
+++ b/tests/event_imageurls.xlsx
@@ -1192,9 +1192,9 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1833,214 +1833,274 @@
       <c r="H35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="n">
+      <c r="A36" s="17" t="n">
         <v>44944.8781752662</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="19" t="s">
         <v>96</v>
       </c>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="17" t="n">
         <v>44944.878976007</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="19" t="s">
         <v>99</v>
       </c>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="n">
+      <c r="A38" s="17" t="n">
         <v>44944.8798733102</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="19" t="s">
         <v>101</v>
       </c>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="n">
+      <c r="A39" s="17" t="n">
         <v>44944.8798959375</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="19" t="s">
         <v>103</v>
       </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="n">
+      <c r="A40" s="17" t="n">
         <v>44944.8842240509</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="19" t="s">
         <v>106</v>
       </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="n">
+      <c r="A41" s="17" t="n">
         <v>44944.8864546991</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="19" t="s">
         <v>109</v>
       </c>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="n">
+      <c r="A42" s="17" t="n">
         <v>44944.8875128125</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="19" t="s">
         <v>112</v>
       </c>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="n">
+      <c r="A43" s="17" t="n">
         <v>44944.887963831</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="19" t="s">
         <v>115</v>
       </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="n">
+      <c r="A44" s="17" t="n">
         <v>44944.8901057986</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="19" t="s">
         <v>117</v>
       </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="n">
+      <c r="A45" s="17" t="n">
         <v>44944.8905932292</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="n">
+      <c r="A46" s="17" t="n">
         <v>44944.8918059144</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="19" t="s">
         <v>121</v>
       </c>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="n">
+      <c r="A47" s="17" t="n">
         <v>44944.9017064468</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="19" t="s">
         <v>124</v>
       </c>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="n">
+      <c r="A48" s="17" t="n">
         <v>44944.9043996181</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="19" t="s">
         <v>126</v>
       </c>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="10" t="n">
+      <c r="A49" s="17" t="n">
         <v>44944.9121669676</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="19" t="s">
         <v>129</v>
       </c>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="n">
+      <c r="A50" s="17" t="n">
         <v>44944.9160223032</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="19" t="s">
         <v>132</v>
       </c>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="n">

</xml_diff>

<commit_message>
feat: added image upload script
</commit_message>
<xml_diff>
--- a/tests/event_imageurls.xlsx
+++ b/tests/event_imageurls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="303">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -896,6 +896,39 @@
   </si>
   <si>
     <t xml:space="preserve">https://drive.google.com/open?id=11qYikTFkogaNSETzO16e50Fxuic8qk9Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Riviera India Quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBQC- VIT Quiz Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/open?id=1AuLECf1up_CDoWB08EN-J0zdjxSdtJ6i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Riviera MELA Quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/open?id=1NH7egQgq9o9rcFjuoEPdNZU13LI-1dqk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Riviera Fandom Quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/open?id=18LjvbgrWNoXAPUoI_HV4W-Ijyomrzipz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Riviera Sports Quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/open?id=1fwb8CEV2yyuAU7rJKe1FRCqr5G5pF2No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Riviera General Quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://drive.google.com/open?id=1K6Vog1qE-tN2fIqVH8Wji_QLpQ0e8rZ_</t>
   </si>
 </sst>
 </file>
@@ -906,7 +939,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -931,28 +964,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -967,7 +978,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -976,20 +987,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA7500"/>
+        <fgColor rgb="FFFFBF00"/>
         <bgColor rgb="FFFF8000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFEA7500"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1027,12 +1044,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1044,71 +1073,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1166,9 +1179,9 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF8000"/>
-      <rgbColor rgb="FFEA7500"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -1189,1814 +1202,1897 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+      <c r="A2" s="2" t="n">
         <v>44944.7934092361</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
+      <c r="A3" s="2" t="n">
         <v>44944.8080016898</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="2" t="n">
         <v>44944.8170711574</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="2" t="n">
         <v>44944.8375656944</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="2" t="n">
         <v>44944.8391739005</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="2" t="n">
         <v>44944.8398078819</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="2" t="n">
         <v>44944.8408987732</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="2" t="n">
         <v>44944.8423293171</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="2" t="n">
         <v>44944.8489307176</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="2" t="n">
         <v>44944.8503160532</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="2" t="n">
         <v>44944.8508571181</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="2" t="n">
         <v>44944.8513970718</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="2" t="n">
         <v>44944.8515471759</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="2" t="n">
         <v>44944.8525725579</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="2" t="n">
         <v>44944.85700375</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="2" t="n">
         <v>44944.8578956597</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="2" t="n">
         <v>44944.8584218056</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="2" t="n">
         <v>44944.868470706</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="2" t="n">
         <v>44944.868923669</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="n">
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
         <v>44944.8699660532</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="n">
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
         <v>44944.8703911458</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="n">
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
         <v>44944.8709897106</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="n">
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
         <v>44944.8717539815</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="n">
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="n">
         <v>44944.8717665972</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="n">
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
         <v>44944.8722108218</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="n">
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="n">
         <v>44944.8723340857</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="n">
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="n">
         <v>44944.8728390857</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="n">
+      <c r="A29" s="2" t="n">
         <v>44944.8735783218</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="n">
+      <c r="A30" s="2" t="n">
         <v>44944.8748265394</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="n">
+      <c r="A31" s="2" t="n">
         <v>44944.8757384838</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="n">
+      <c r="A32" s="2" t="n">
         <v>44944.8759675232</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="n">
+      <c r="A33" s="2" t="n">
         <v>44944.8769399653</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="n">
+      <c r="A34" s="2" t="n">
         <v>44944.8771110417</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="n">
+      <c r="A35" s="2" t="n">
         <v>44944.8774606019</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="n">
+      <c r="A36" s="2" t="n">
         <v>44944.8781752662</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="n">
+      <c r="A37" s="2" t="n">
         <v>44944.878976007</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="n">
+      <c r="A38" s="2" t="n">
         <v>44944.8798733102</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="17" t="n">
+      <c r="A39" s="2" t="n">
         <v>44944.8798959375</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="n">
+      <c r="A40" s="2" t="n">
         <v>44944.8842240509</v>
       </c>
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="17" t="n">
+      <c r="A41" s="2" t="n">
         <v>44944.8864546991</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="17" t="n">
+      <c r="A42" s="2" t="n">
         <v>44944.8875128125</v>
       </c>
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="17" t="n">
+      <c r="A43" s="2" t="n">
         <v>44944.887963831</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="n">
+      <c r="A44" s="2" t="n">
         <v>44944.8901057986</v>
       </c>
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="17" t="n">
+      <c r="A45" s="2" t="n">
         <v>44944.8905932292</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="n">
+      <c r="A46" s="2" t="n">
         <v>44944.8918059144</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="17" t="n">
+      <c r="A47" s="2" t="n">
         <v>44944.9017064468</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="17" t="n">
+      <c r="A48" s="2" t="n">
         <v>44944.9043996181</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="17" t="n">
+      <c r="A49" s="2" t="n">
         <v>44944.9121669676</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="17" t="n">
+      <c r="A50" s="2" t="n">
         <v>44944.9160223032</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="n">
+      <c r="A51" s="2" t="n">
         <v>44944.918583831</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="n">
+      <c r="A52" s="2" t="n">
         <v>44944.9235236343</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="n">
+      <c r="A53" s="4" t="n">
         <v>44944.9288482523</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="6" t="s">
         <v>140</v>
       </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="n">
+      <c r="A54" s="4" t="n">
         <v>44944.9290828241</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="6" t="s">
         <v>143</v>
       </c>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="n">
+      <c r="A55" s="4" t="n">
         <v>44944.9365657176</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="6" t="s">
         <v>146</v>
       </c>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="n">
+      <c r="A56" s="2" t="n">
         <v>44944.9441115046</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="n">
+      <c r="A57" s="4" t="n">
         <v>44944.9443059375</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="6" t="s">
         <v>150</v>
       </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="n">
+      <c r="A58" s="4" t="n">
         <v>44944.9455482292</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="6" t="s">
         <v>153</v>
       </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="n">
+      <c r="A59" s="4" t="n">
         <v>44944.9459856482</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="6" t="s">
         <v>155</v>
       </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="n">
+      <c r="A60" s="4" t="n">
         <v>44944.9528217477</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="6" t="s">
         <v>157</v>
       </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="n">
+      <c r="A61" s="4" t="n">
         <v>44944.9550264699</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="6" t="s">
         <v>160</v>
       </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="n">
+      <c r="A62" s="4" t="n">
         <v>44944.9580266551</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="6" t="s">
         <v>163</v>
       </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="n">
+      <c r="A63" s="4" t="n">
         <v>44944.9660910301</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="6" t="s">
         <v>166</v>
       </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="n">
+      <c r="A64" s="8" t="n">
         <v>44944.9746368519</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B64" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="10" t="s">
         <v>169</v>
       </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="n">
+      <c r="A65" s="12" t="n">
         <v>44944.9752242477</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D65" s="14" t="s">
         <v>172</v>
       </c>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="n">
+      <c r="A66" s="12" t="n">
         <v>44944.9756019097</v>
       </c>
-      <c r="B66" s="11" t="s">
+      <c r="B66" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="14" t="s">
         <v>175</v>
       </c>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="n">
+      <c r="A67" s="12" t="n">
         <v>44944.9760209954</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="14" t="s">
         <v>178</v>
       </c>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="n">
+      <c r="A68" s="12" t="n">
         <v>44944.9771058796</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="14" t="s">
         <v>181</v>
       </c>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="n">
+      <c r="A69" s="12" t="n">
         <v>44944.9778847454</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="14" t="s">
         <v>183</v>
       </c>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="n">
+      <c r="A70" s="12" t="n">
         <v>44944.979121713</v>
       </c>
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="14" t="s">
         <v>185</v>
       </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10" t="n">
+      <c r="A71" s="12" t="n">
         <v>44944.9794387384</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="D71" s="14" t="s">
         <v>188</v>
       </c>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="n">
+      <c r="A72" s="12" t="n">
         <v>44944.9794535185</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D72" s="14" t="s">
         <v>190</v>
       </c>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10" t="n">
+      <c r="A73" s="12" t="n">
         <v>44944.9797433681</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D73" s="12" t="s">
+      <c r="D73" s="14" t="s">
         <v>192</v>
       </c>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="10" t="n">
+      <c r="A74" s="12" t="n">
         <v>44944.9814236343</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="D74" s="12" t="s">
+      <c r="D74" s="14" t="s">
         <v>194</v>
       </c>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="10" t="n">
+      <c r="A75" s="12" t="n">
         <v>44944.9815203472</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="D75" s="12" t="s">
+      <c r="D75" s="14" t="s">
         <v>197</v>
       </c>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="10" t="n">
+      <c r="A76" s="12" t="n">
         <v>44944.9822379977</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="C76" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D76" s="14" t="s">
         <v>199</v>
       </c>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="10" t="n">
+      <c r="A77" s="12" t="n">
         <v>44944.9823285301</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="14" t="s">
         <v>202</v>
       </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="10" t="n">
+      <c r="A78" s="12" t="n">
         <v>44944.9841382292</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="14" t="s">
         <v>205</v>
       </c>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="n">
+      <c r="A79" s="12" t="n">
         <v>44944.9846979282</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="10" t="n">
+      <c r="A80" s="12" t="n">
         <v>44944.9849382523</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="14" t="s">
         <v>211</v>
       </c>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="10" t="n">
+      <c r="A81" s="12" t="n">
         <v>44944.988722662</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="14" t="s">
         <v>213</v>
       </c>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="10" t="n">
+      <c r="A82" s="2" t="n">
         <v>44944.9889388773</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D82" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="10" t="n">
+      <c r="A83" s="2" t="n">
         <v>44944.9911239815</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="10" t="n">
+      <c r="A84" s="2" t="n">
         <v>44944.9934737384</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="n">
+      <c r="A85" s="2" t="n">
         <v>44944.9947862153</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="C85" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="10" t="n">
+      <c r="A86" s="16" t="n">
         <v>44944.9950557292</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="C86" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="18" t="s">
         <v>225</v>
       </c>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="10" t="n">
+      <c r="A87" s="2" t="n">
         <v>44944.9951731944</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C87" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D87" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="10" t="n">
+      <c r="A88" s="2" t="n">
         <v>44944.9954082986</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C88" s="11" t="s">
+      <c r="C88" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D88" s="12" t="s">
+      <c r="D88" s="3" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="10" t="n">
+      <c r="A89" s="16" t="n">
         <v>44944.9955777199</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D89" s="12" t="s">
+      <c r="D89" s="18" t="s">
         <v>233</v>
       </c>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="10" t="n">
+      <c r="A90" s="2" t="n">
         <v>44944.9956394676</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="10" t="n">
+      <c r="A91" s="16" t="n">
         <v>44944.9957084028</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="18" t="s">
         <v>238</v>
       </c>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="10" t="n">
+      <c r="A92" s="16" t="n">
         <v>44944.9960441551</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="18" t="s">
         <v>240</v>
       </c>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="10" t="n">
+      <c r="A93" s="16" t="n">
         <v>44944.9968107639</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="18" t="s">
         <v>242</v>
       </c>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10" t="n">
+      <c r="A94" s="16" t="n">
         <v>44944.9968666782</v>
       </c>
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="18" t="s">
         <v>244</v>
       </c>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10" t="n">
+      <c r="A95" s="16" t="n">
         <v>44944.9972932523</v>
       </c>
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="C95" s="11" t="s">
+      <c r="C95" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D95" s="12" t="s">
+      <c r="D95" s="18" t="s">
         <v>246</v>
       </c>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="10" t="n">
+      <c r="A96" s="2" t="n">
         <v>44944.997554375</v>
       </c>
-      <c r="B96" s="11" t="s">
+      <c r="B96" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="10" t="n">
+      <c r="A97" s="16" t="n">
         <v>44944.9979558565</v>
       </c>
-      <c r="B97" s="11" t="s">
+      <c r="B97" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="C97" s="11" t="s">
+      <c r="C97" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" s="18" t="s">
         <v>250</v>
       </c>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="19"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="10" t="n">
+      <c r="A98" s="2" t="n">
         <v>44944.9980330324</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D98" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="10" t="n">
+      <c r="A99" s="2" t="n">
         <v>44945.0181884144</v>
       </c>
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C99" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D99" s="12" t="s">
+      <c r="D99" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="10" t="n">
+      <c r="A100" s="12" t="n">
         <v>44945.3630594329</v>
       </c>
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C100" s="11" t="s">
+      <c r="C100" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="14" t="s">
         <v>258</v>
       </c>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="10" t="n">
+      <c r="A101" s="12" t="n">
         <v>44945.3636574074</v>
       </c>
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="C101" s="11" t="s">
+      <c r="C101" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D101" s="14" t="s">
         <v>260</v>
       </c>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="10" t="n">
+      <c r="A102" s="12" t="n">
         <v>44945.3641343403</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D102" s="14" t="s">
         <v>262</v>
       </c>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="10" t="n">
+      <c r="A103" s="12" t="n">
         <v>44945.3648879398</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D103" s="14" t="s">
         <v>264</v>
       </c>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="10" t="n">
+      <c r="A104" s="12" t="n">
         <v>44945.3658216204</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D104" s="14" t="s">
         <v>267</v>
       </c>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="10" t="n">
+      <c r="A105" s="12" t="n">
         <v>44945.3664043287</v>
       </c>
-      <c r="B105" s="11" t="s">
+      <c r="B105" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C105" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D105" s="12" t="s">
+      <c r="D105" s="14" t="s">
         <v>269</v>
       </c>
+      <c r="E105" s="15"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="15"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="10" t="n">
+      <c r="A106" s="12" t="n">
         <v>44945.3668175347</v>
       </c>
-      <c r="B106" s="11" t="s">
+      <c r="B106" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D106" s="14" t="s">
         <v>271</v>
       </c>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="15"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="10" t="n">
+      <c r="A107" s="12" t="n">
         <v>44945.4953859838</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="10" t="n">
+      <c r="A108" s="12" t="n">
         <v>44945.4960377083</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="14" t="s">
         <v>276</v>
       </c>
+      <c r="E108" s="15"/>
+      <c r="F108" s="15"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="15"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="10" t="n">
+      <c r="A109" s="12" t="n">
         <v>44945.5184475</v>
       </c>
-      <c r="B109" s="11" t="s">
+      <c r="B109" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="C109" s="11" t="s">
+      <c r="C109" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D109" s="14" t="s">
         <v>279</v>
       </c>
+      <c r="E109" s="15"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="15"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="10" t="n">
+      <c r="A110" s="12" t="n">
         <v>44945.5200421296</v>
       </c>
-      <c r="B110" s="11" t="s">
+      <c r="B110" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="D110" s="12" t="s">
+      <c r="D110" s="14" t="s">
         <v>281</v>
       </c>
+      <c r="E110" s="15"/>
+      <c r="F110" s="15"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="10" t="n">
+      <c r="A111" s="12" t="n">
         <v>44945.6005736227</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="D111" s="12" t="s">
+      <c r="D111" s="14" t="s">
         <v>284</v>
       </c>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="15"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="10" t="n">
+      <c r="A112" s="12" t="n">
         <v>44945.6050966319</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="D112" s="14" t="s">
         <v>286</v>
       </c>
+      <c r="E112" s="15"/>
+      <c r="F112" s="15"/>
+      <c r="G112" s="15"/>
+      <c r="H112" s="15"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="10" t="n">
+      <c r="A113" s="12" t="n">
         <v>44945.6168560764</v>
       </c>
-      <c r="B113" s="11" t="s">
+      <c r="B113" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="C113" s="11" t="s">
+      <c r="C113" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="D113" s="12" t="s">
+      <c r="D113" s="14" t="s">
         <v>288</v>
       </c>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="15"/>
+      <c r="H113" s="15"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="10" t="n">
+      <c r="A114" s="12" t="n">
         <v>44945.6541967477</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="14" t="s">
         <v>291</v>
       </c>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+      <c r="H114" s="15"/>
+    </row>
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="12" t="n">
+        <v>44945.8161554514</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
+      <c r="H115" s="15"/>
+    </row>
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="12" t="n">
+        <v>44945.8168649653</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+      <c r="H116" s="15"/>
+    </row>
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="12" t="n">
+        <v>44945.8176363426</v>
+      </c>
+      <c r="B117" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="15"/>
+    </row>
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="12" t="n">
+        <v>44945.8181844329</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+    </row>
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="12" t="n">
+        <v>44945.8186958102</v>
+      </c>
+      <c r="B119" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+    </row>
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="15"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+      <c r="H120" s="15"/>
+    </row>
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A121" s="15"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3113,6 +3209,11 @@
     <hyperlink ref="D112" r:id="rId111" display="https://drive.google.com/open?id=1Vng3-VufSSIiw7TlwPt_BcVdHS1ZBg_i"/>
     <hyperlink ref="D113" r:id="rId112" display="https://drive.google.com/open?id=1kTQmyNpzcVnATZ6MXoMwJ3bsYmmcV_SH"/>
     <hyperlink ref="D114" r:id="rId113" display="https://drive.google.com/open?id=11qYikTFkogaNSETzO16e50Fxuic8qk9Y"/>
+    <hyperlink ref="D115" r:id="rId114" display="https://drive.google.com/open?id=1AuLECf1up_CDoWB08EN-J0zdjxSdtJ6i"/>
+    <hyperlink ref="D116" r:id="rId115" display="https://drive.google.com/open?id=1NH7egQgq9o9rcFjuoEPdNZU13LI-1dqk"/>
+    <hyperlink ref="D117" r:id="rId116" display="https://drive.google.com/open?id=18LjvbgrWNoXAPUoI_HV4W-Ijyomrzipz"/>
+    <hyperlink ref="D118" r:id="rId117" display="https://drive.google.com/open?id=1fwb8CEV2yyuAU7rJKe1FRCqr5G5pF2No"/>
+    <hyperlink ref="D119" r:id="rId118" display="https://drive.google.com/open?id=1K6Vog1qE-tN2fIqVH8Wji_QLpQ0e8rZ_"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>